<commit_message>
convert from xlsx to json + EXO mail flow rules
</commit_message>
<xml_diff>
--- a/InformationBarriers/InfoBarriers-PowerShellGenerator-clean.xlsx
+++ b/InformationBarriers/InfoBarriers-PowerShellGenerator-clean.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22410"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="42" documentId="8_{D58670C2-4702-49D7-8FF5-B9A6F248DF0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6B246742-B4CB-4110-B4D9-B5A5B4ABCF54}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F9D771-5564-4075-BF63-ED3C14F688D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{DB72A67B-08E2-4272-83B0-820083636442}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{DB72A67B-08E2-4272-83B0-820083636442}"/>
   </bookViews>
   <sheets>
-    <sheet name="Information Barriers" sheetId="10" r:id="rId1"/>
+    <sheet name="OrganizationSegments" sheetId="10" r:id="rId1"/>
+    <sheet name="Policies" sheetId="11" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>-eq</t>
   </si>
@@ -85,6 +86,18 @@
   </si>
   <si>
     <t>ib-administrasjon</t>
+  </si>
+  <si>
+    <t>elever-skole1, elever-skole2</t>
+  </si>
+  <si>
+    <t>AllowedSegements</t>
+  </si>
+  <si>
+    <t>administrasjon, lerere-skole2</t>
+  </si>
+  <si>
+    <t>administrasjon, lerere-skole1</t>
   </si>
 </sst>
 </file>
@@ -108,9 +121,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -145,21 +156,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -472,23 +478,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F5DD102-B566-436D-A000-AD510D0A7606}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.07421875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="21.265625" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="19.3984375" customWidth="1"/>
-    <col min="4" max="5" width="20.3984375" customWidth="1"/>
-    <col min="6" max="6" width="15.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.23046875" customWidth="1"/>
+    <col min="2" max="2" width="19.69140625" customWidth="1"/>
+    <col min="3" max="3" width="19.3828125" customWidth="1"/>
+    <col min="4" max="4" width="20.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -501,15 +505,8 @@
       <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -522,15 +519,8 @@
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -543,15 +533,8 @@
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -564,15 +547,8 @@
       <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -585,15 +561,8 @@
       <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -606,63 +575,10 @@
       <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="E10" s="6"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C11" s="4"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C9" xr:uid="{9505328C-C523-4DE6-9987-633D5D59AE85}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C6" xr:uid="{9505328C-C523-4DE6-9987-633D5D59AE85}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -671,26 +587,83 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7B4146-67BB-4C5C-931A-6314580B8BC8}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="20.4609375" customWidth="1"/>
+    <col min="2" max="2" width="29.15234375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="0eddaf13-8b9c-491d-8989-96467b25f0fe" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006AB3688720243E4CA5A3AB4E1E5487D7" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0a7e63862b3d41b2389f26a9f2c0dc08">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="33027751-b62e-4e62-a476-7ad2776d8388" xmlns:ns3="0eddaf13-8b9c-491d-8989-96467b25f0fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7cc73ac57a48faae2ee8776b62d90698" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -936,33 +909,26 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="0eddaf13-8b9c-491d-8989-96467b25f0fe" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D051598-B463-4AB1-AA71-3BF6A00F46C6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="33027751-b62e-4e62-a476-7ad2776d8388"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="0eddaf13-8b9c-491d-8989-96467b25f0fe"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDAAE0C7-FC0A-4B41-9435-17537DF3F14A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6C5DA2E-B93E-4E07-B2D1-8AB0F7E4B5A1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -980,4 +946,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D051598-B463-4AB1-AA71-3BF6A00F46C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="33027751-b62e-4e62-a476-7ad2776d8388"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="0eddaf13-8b9c-491d-8989-96467b25f0fe"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDAAE0C7-FC0A-4B41-9435-17537DF3F14A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>